<commit_message>
got rid of dupicates and clean daat
</commit_message>
<xml_diff>
--- a/data/modified_file.xlsx
+++ b/data/modified_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Oklahoma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D44301-7A3E-274B-9B30-34E9E552F0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96896048-4F3D-9A4D-BD38-1CD1299E6C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="745">
   <si>
     <t>Organization</t>
   </si>
@@ -2237,12 +2237,45 @@
   <si>
     <t>2nd Grade Students / Youth, 3rd Grade Students / Youth, 4th Grade Students / Youth, 5th Grade Students / Youth, 6th Grade Students / Youth, 7th Grade Students / Youth, 8th Grade Students / Youth, 9th Grade Students / Youth, 10th Grade Students / Youth, 11th Grade Students / Youth, 12th Grade Students / Youth, Pre-Service Educators/College Students, Teachers/Administrators, Informal Educators, General Public/Family, Senior Citizens, Adults</t>
   </si>
+  <si>
+    <t>Keep Oklahoma Beautiful, Inc.</t>
+  </si>
+  <si>
+    <t>Keep Oklahoma Beautiful encourages high school and college students to take action in the fight against litter and illegal dumping in Oklahoma! We challenge students to tackle this issue in a 25-45 second video clip that conveys to all citizens of Oklahoma that littering is costly, deplorable, illegal, and just downright wrong. In addition to the video, students are required to submit a short essay detailing research conducted for their video.</t>
+  </si>
+  <si>
+    <t>Classroom volunteers/presenters,Curriculum &amp; instructional materials,Field trips</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Conservation (Wildlife/Habitat),Waste</t>
+  </si>
+  <si>
+    <t>State Standards (Write in Other),Other</t>
+  </si>
+  <si>
+    <t>9th Grade Students / Youth,10th Grade Students / Youth,11th Grade Students / Youth,12th Grade Students / Youth,Pre-Service Educators/College Students</t>
+  </si>
+  <si>
+    <t>This is not our core focus, but we serve a diverse spectrum of schools and/or students.</t>
+  </si>
+  <si>
+    <t>Post-program survey only,External evaluation partner,Rubrics for student projects/presentations</t>
+  </si>
+  <si>
+    <t>On K-12 school campus,Virtual</t>
+  </si>
+  <si>
+    <t>During school day,After school,Evenings,Weekends</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2254,6 +2287,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2292,7 +2331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2303,6 +2342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2607,13 +2647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="47.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -2697,7 +2737,7 @@
     <col min="83" max="83" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:83" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6645,10 +6685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BG51"/>
+  <dimension ref="A1:BG52"/>
   <sheetViews>
-    <sheetView zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="BG1" sqref="BG1:BG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6706,7 +6746,7 @@
     <col min="51" max="51" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="30.5" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="21" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.6640625" customWidth="1"/>
     <col min="55" max="55" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="23" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="18.5" bestFit="1" customWidth="1"/>
@@ -7035,87 +7075,92 @@
         <v>493</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="192" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="D4">
-        <v>23760</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="I4" t="s">
-        <v>497</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="D4" s="4">
+        <v>23764</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="V4">
-        <v>5095</v>
-      </c>
-      <c r="W4">
-        <v>49</v>
-      </c>
-      <c r="X4">
-        <v>988</v>
-      </c>
-      <c r="Y4">
-        <v>36</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="V4" s="4">
+        <v>3062</v>
+      </c>
+      <c r="W4" s="4">
+        <v>31</v>
+      </c>
+      <c r="X4" s="4">
+        <v>620</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>19</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AA4" t="s">
-        <v>503</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AA4" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>482</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>483</v>
-      </c>
     </row>
-    <row r="5" spans="1:59" ht="128" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="192" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -7123,13 +7168,13 @@
         <v>190</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="D5">
-        <v>23762</v>
+        <v>23760</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="I5" t="s">
         <v>497</v>
@@ -7147,7 +7192,7 @@
         <v>475</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>502</v>
@@ -7156,16 +7201,16 @@
         <v>478</v>
       </c>
       <c r="V5">
-        <v>573</v>
+        <v>5095</v>
       </c>
       <c r="W5">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="X5">
-        <v>660</v>
+        <v>988</v>
       </c>
       <c r="Y5">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="Z5" t="s">
         <v>160</v>
@@ -7195,7 +7240,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="144" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -7203,13 +7248,13 @@
         <v>190</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D6">
-        <v>23764</v>
+        <v>23762</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I6" t="s">
         <v>497</v>
@@ -7227,7 +7272,7 @@
         <v>475</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>502</v>
@@ -7236,16 +7281,16 @@
         <v>478</v>
       </c>
       <c r="V6">
-        <v>3062</v>
+        <v>573</v>
       </c>
       <c r="W6">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X6">
-        <v>620</v>
+        <v>660</v>
       </c>
       <c r="Y6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Z6" t="s">
         <v>160</v>
@@ -7257,7 +7302,7 @@
         <v>504</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="AE6" t="s">
         <v>492</v>
@@ -7275,7 +7320,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="144" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -7283,28 +7328,31 @@
         <v>190</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D7">
-        <v>23768</v>
+        <v>23764</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I7" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>517</v>
+        <v>499</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>500</v>
       </c>
       <c r="Q7" t="s">
         <v>475</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>476</v>
+        <v>511</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>502</v>
@@ -7313,31 +7361,31 @@
         <v>478</v>
       </c>
       <c r="V7">
-        <v>20</v>
+        <v>3062</v>
       </c>
       <c r="W7">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="X7">
-        <v>400</v>
+        <v>620</v>
       </c>
       <c r="Y7">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="Z7" t="s">
         <v>160</v>
       </c>
       <c r="AA7" t="s">
-        <v>490</v>
+        <v>503</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="AE7" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="AI7" t="s">
         <v>198</v>
@@ -7357,52 +7405,49 @@
         <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="D8">
-        <v>24409</v>
+        <v>23768</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="I8" t="s">
-        <v>522</v>
-      </c>
-      <c r="K8" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="Q8" t="s">
         <v>475</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>526</v>
+        <v>476</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>502</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>527</v>
+        <v>478</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X8">
-        <v>31000</v>
+        <v>400</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Z8" t="s">
         <v>160</v>
@@ -7411,16 +7456,16 @@
         <v>490</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="AE8" t="s">
-        <v>492</v>
+        <v>519</v>
       </c>
       <c r="AI8" t="s">
-        <v>481</v>
+        <v>198</v>
       </c>
       <c r="AJ8" t="s">
         <v>482</v>
@@ -7432,7 +7477,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="350" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -7440,31 +7485,31 @@
         <v>246</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="D9">
-        <v>24411</v>
+        <v>24409</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="I9" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="K9" t="s">
         <v>523</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="Q9" t="s">
         <v>475</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>502</v>
@@ -7479,7 +7524,7 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>950</v>
+        <v>31000</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -7497,10 +7542,10 @@
         <v>480</v>
       </c>
       <c r="AE9" t="s">
-        <v>534</v>
+        <v>492</v>
       </c>
       <c r="AI9" t="s">
-        <v>535</v>
+        <v>481</v>
       </c>
       <c r="AJ9" t="s">
         <v>482</v>
@@ -7512,7 +7557,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="192" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="350" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -7520,34 +7565,37 @@
         <v>246</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="D10">
-        <v>24413</v>
+        <v>24411</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="I10" t="s">
-        <v>538</v>
+        <v>531</v>
+      </c>
+      <c r="K10" t="s">
+        <v>523</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="Q10" t="s">
         <v>475</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>501</v>
+        <v>533</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>502</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>478</v>
+        <v>527</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -7556,7 +7604,7 @@
         <v>0</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -7568,13 +7616,13 @@
         <v>490</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="AE10" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="AI10" t="s">
         <v>535</v>
@@ -7589,42 +7637,36 @@
         <v>483</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D11">
-        <v>24509</v>
+        <v>24413</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>274</v>
+        <v>537</v>
       </c>
       <c r="I11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="N11" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
       <c r="Q11" t="s">
         <v>475</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>545</v>
+        <v>501</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>502</v>
@@ -7648,19 +7690,19 @@
         <v>160</v>
       </c>
       <c r="AA11" t="s">
-        <v>546</v>
+        <v>490</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>547</v>
+        <v>505</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>519</v>
       </c>
       <c r="AI11" t="s">
-        <v>198</v>
+        <v>535</v>
       </c>
       <c r="AJ11" t="s">
         <v>482</v>
@@ -7671,67 +7713,76 @@
       <c r="AM11" t="s">
         <v>483</v>
       </c>
-      <c r="BG11" t="s">
-        <v>139</v>
-      </c>
     </row>
-    <row r="12" spans="1:59" ht="240" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="D12">
-        <v>24456</v>
+        <v>24509</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>549</v>
+        <v>274</v>
       </c>
       <c r="I12" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>551</v>
+        <v>138</v>
+      </c>
+      <c r="N12" t="s">
+        <v>542</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>517</v>
+        <v>543</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>544</v>
       </c>
       <c r="Q12" t="s">
         <v>475</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>489</v>
+        <v>502</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>478</v>
       </c>
       <c r="V12">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>7500</v>
+        <v>0</v>
       </c>
       <c r="Y12">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="Z12" t="s">
         <v>160</v>
       </c>
       <c r="AA12" t="s">
-        <v>490</v>
+        <v>546</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>528</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>554</v>
+        <v>138</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>547</v>
       </c>
       <c r="AI12" t="s">
         <v>198</v>
@@ -7745,70 +7796,67 @@
       <c r="AM12" t="s">
         <v>483</v>
       </c>
+      <c r="BG12" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="13" spans="1:59" ht="380" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="240" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>83</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="D13">
-        <v>23740</v>
+        <v>24456</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="I13" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="Q13" t="s">
         <v>475</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>560</v>
+        <v>489</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="W13">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="X13">
-        <v>4000</v>
+        <v>7500</v>
       </c>
       <c r="Y13">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="Z13" t="s">
         <v>160</v>
       </c>
       <c r="AA13" t="s">
-        <v>561</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="AE13" t="s">
-        <v>492</v>
+        <v>554</v>
       </c>
       <c r="AI13" t="s">
         <v>198</v>
@@ -7823,7 +7871,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="335" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="380" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -7831,64 +7879,61 @@
         <v>283</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="D14">
-        <v>23742</v>
+        <v>23740</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="I14" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="Q14" t="s">
         <v>475</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>502</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>478</v>
+        <v>560</v>
       </c>
       <c r="V14">
         <v>0</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Z14" t="s">
         <v>160</v>
       </c>
       <c r="AA14" t="s">
-        <v>490</v>
+        <v>561</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>568</v>
+        <v>479</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="AE14" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="AI14" t="s">
         <v>198</v>
@@ -7903,7 +7948,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="335" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -7911,19 +7956,19 @@
         <v>283</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="D15">
-        <v>23744</v>
+        <v>23742</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="I15" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>517</v>
@@ -7932,7 +7977,7 @@
         <v>475</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>476</v>
+        <v>567</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>502</v>
@@ -7959,7 +8004,7 @@
         <v>490</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>528</v>
+        <v>568</v>
       </c>
       <c r="AC15" s="3" t="s">
         <v>138</v>
@@ -7982,34 +8027,28 @@
       <c r="AM15" t="s">
         <v>483</v>
       </c>
-      <c r="BG15" t="s">
-        <v>574</v>
-      </c>
     </row>
-    <row r="16" spans="1:59" ht="144" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>83</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>494</v>
+        <v>570</v>
       </c>
       <c r="D16">
-        <v>25119</v>
+        <v>23744</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I16" t="s">
-        <v>576</v>
-      </c>
-      <c r="K16" t="s">
-        <v>523</v>
+        <v>572</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>517</v>
@@ -8018,7 +8057,7 @@
         <v>475</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>578</v>
+        <v>476</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>502</v>
@@ -8033,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="X16">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -8042,16 +8081,19 @@
         <v>160</v>
       </c>
       <c r="AA16" t="s">
-        <v>579</v>
+        <v>490</v>
       </c>
       <c r="AB16" s="3" t="s">
         <v>528</v>
       </c>
       <c r="AC16" s="3" t="s">
-        <v>580</v>
+        <v>138</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>569</v>
       </c>
       <c r="AE16" t="s">
-        <v>554</v>
+        <v>519</v>
       </c>
       <c r="AI16" t="s">
         <v>198</v>
@@ -8066,10 +8108,10 @@
         <v>483</v>
       </c>
       <c r="BG16" t="s">
-        <v>139</v>
+        <v>574</v>
       </c>
     </row>
-    <row r="17" spans="1:59" ht="176" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:59" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -8077,31 +8119,31 @@
         <v>284</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>581</v>
+        <v>494</v>
       </c>
       <c r="D17">
-        <v>25121</v>
+        <v>25119</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="I17" t="s">
-        <v>583</v>
+        <v>576</v>
+      </c>
+      <c r="K17" t="s">
+        <v>523</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>585</v>
+        <v>517</v>
       </c>
       <c r="Q17" t="s">
         <v>475</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>502</v>
@@ -8113,10 +8155,10 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -8128,13 +8170,13 @@
         <v>579</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>479</v>
+        <v>528</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>480</v>
+        <v>580</v>
       </c>
       <c r="AE17" t="s">
-        <v>492</v>
+        <v>554</v>
       </c>
       <c r="AI17" t="s">
         <v>198</v>
@@ -8152,7 +8194,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:59" ht="112" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:59" ht="176" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -8160,31 +8202,31 @@
         <v>284</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D18">
-        <v>25123</v>
+        <v>25121</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="I18" t="s">
-        <v>589</v>
-      </c>
-      <c r="K18" t="s">
-        <v>523</v>
+        <v>583</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>517</v>
+        <v>499</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>585</v>
       </c>
       <c r="Q18" t="s">
         <v>475</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="T18" s="3" t="s">
         <v>502</v>
@@ -8196,10 +8238,10 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="X18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y18">
         <v>0</v>
@@ -8208,7 +8250,7 @@
         <v>160</v>
       </c>
       <c r="AA18" t="s">
-        <v>490</v>
+        <v>579</v>
       </c>
       <c r="AB18" s="3" t="s">
         <v>479</v>
@@ -8217,7 +8259,7 @@
         <v>480</v>
       </c>
       <c r="AE18" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="AI18" t="s">
         <v>198</v>
@@ -8231,8 +8273,11 @@
       <c r="AM18" t="s">
         <v>483</v>
       </c>
+      <c r="BG18" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="19" spans="1:59" ht="350" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:59" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -8240,13 +8285,13 @@
         <v>284</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D19">
-        <v>25125</v>
+        <v>25123</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="I19" t="s">
         <v>589</v>
@@ -8255,19 +8300,16 @@
         <v>523</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>595</v>
+        <v>517</v>
       </c>
       <c r="Q19" t="s">
         <v>475</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>502</v>
@@ -8297,7 +8339,7 @@
         <v>479</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="AE19" t="s">
         <v>519</v>
@@ -8314,70 +8356,79 @@
       <c r="AM19" t="s">
         <v>483</v>
       </c>
-      <c r="BG19" t="s">
-        <v>139</v>
-      </c>
     </row>
-    <row r="20" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:59" ht="350" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="D20">
-        <v>23735</v>
+        <v>25125</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="I20" t="s">
-        <v>599</v>
+        <v>589</v>
+      </c>
+      <c r="K20" t="s">
+        <v>523</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>601</v>
+        <v>499</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>595</v>
       </c>
       <c r="Q20" t="s">
         <v>475</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>478</v>
       </c>
       <c r="V20">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="X20">
-        <v>280</v>
+        <v>1000</v>
       </c>
       <c r="Y20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Z20" t="s">
         <v>160</v>
       </c>
       <c r="AA20" t="s">
-        <v>579</v>
+        <v>490</v>
       </c>
       <c r="AB20" s="3" t="s">
         <v>479</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="AE20" t="s">
         <v>519</v>
       </c>
       <c r="AI20" t="s">
-        <v>603</v>
+        <v>198</v>
       </c>
       <c r="AJ20" t="s">
         <v>482</v>
@@ -8388,76 +8439,70 @@
       <c r="AM20" t="s">
         <v>483</v>
       </c>
+      <c r="BG20" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="21" spans="1:59" ht="128" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="D21">
-        <v>23777</v>
+        <v>23735</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="I21" t="s">
-        <v>541</v>
-      </c>
-      <c r="K21" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="Q21" t="s">
-        <v>609</v>
+        <v>475</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="U21" s="3" t="s">
-        <v>560</v>
+        <v>602</v>
       </c>
       <c r="V21">
-        <v>7</v>
+        <v>3000</v>
       </c>
       <c r="W21">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="X21">
-        <v>2500</v>
+        <v>280</v>
       </c>
       <c r="Y21">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="Z21" t="s">
         <v>160</v>
       </c>
       <c r="AA21" t="s">
-        <v>611</v>
+        <v>579</v>
       </c>
       <c r="AB21" s="3" t="s">
         <v>479</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>612</v>
+        <v>480</v>
       </c>
       <c r="AE21" t="s">
-        <v>554</v>
+        <v>519</v>
       </c>
       <c r="AI21" t="s">
-        <v>198</v>
+        <v>603</v>
       </c>
       <c r="AJ21" t="s">
         <v>482</v>
@@ -8468,82 +8513,76 @@
       <c r="AM21" t="s">
         <v>483</v>
       </c>
-      <c r="BG21" t="s">
-        <v>613</v>
-      </c>
     </row>
-    <row r="22" spans="1:59" ht="365" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:59" ht="128" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="D22">
-        <v>24416</v>
+        <v>23777</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="I22" t="s">
-        <v>616</v>
-      </c>
-      <c r="J22" t="s">
-        <v>617</v>
+        <v>541</v>
       </c>
       <c r="K22" t="s">
-        <v>523</v>
+        <v>606</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="N22" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="Q22" t="s">
-        <v>475</v>
+        <v>609</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>621</v>
+        <v>610</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>560</v>
       </c>
       <c r="V22">
-        <v>8000</v>
+        <v>7</v>
       </c>
       <c r="W22">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="X22">
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="Z22" t="s">
         <v>160</v>
       </c>
       <c r="AA22" t="s">
-        <v>490</v>
+        <v>611</v>
       </c>
       <c r="AB22" s="3" t="s">
         <v>479</v>
       </c>
       <c r="AC22" s="3" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="AE22" t="s">
-        <v>492</v>
+        <v>554</v>
       </c>
       <c r="AI22" t="s">
-        <v>481</v>
+        <v>198</v>
       </c>
       <c r="AJ22" t="s">
         <v>482</v>
@@ -8555,7 +8594,7 @@
         <v>483</v>
       </c>
       <c r="BG22" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
     </row>
     <row r="23" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -8566,29 +8605,35 @@
         <v>326</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="D23">
-        <v>24418</v>
+        <v>24416</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="I23" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="J23" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="K23" t="s">
-        <v>628</v>
+        <v>523</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="N23" t="s">
         <v>619</v>
       </c>
+      <c r="O23" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>620</v>
+      </c>
       <c r="Q23" t="s">
         <v>475</v>
       </c>
@@ -8596,13 +8641,13 @@
         <v>621</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -8623,7 +8668,7 @@
         <v>492</v>
       </c>
       <c r="AI23" t="s">
-        <v>535</v>
+        <v>481</v>
       </c>
       <c r="AJ23" t="s">
         <v>482</v>
@@ -8633,6 +8678,9 @@
       </c>
       <c r="AM23" t="s">
         <v>483</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="24" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -8643,35 +8691,29 @@
         <v>326</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="D24">
-        <v>24420</v>
+        <v>24418</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="I24" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="J24" t="s">
         <v>627</v>
       </c>
       <c r="K24" t="s">
-        <v>523</v>
+        <v>628</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>618</v>
+        <v>629</v>
       </c>
       <c r="N24" t="s">
         <v>619</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="Q24" t="s">
         <v>475</v>
       </c>
@@ -8679,13 +8721,13 @@
         <v>621</v>
       </c>
       <c r="V24">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="W24">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="X24">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="Y24">
         <v>0</v>
@@ -8706,7 +8748,7 @@
         <v>492</v>
       </c>
       <c r="AI24" t="s">
-        <v>481</v>
+        <v>535</v>
       </c>
       <c r="AJ24" t="s">
         <v>482</v>
@@ -8716,9 +8758,6 @@
       </c>
       <c r="AM24" t="s">
         <v>483</v>
-      </c>
-      <c r="BG24" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="25" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -8729,16 +8768,16 @@
         <v>326</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D25">
-        <v>24422</v>
+        <v>24420</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="I25" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="J25" t="s">
         <v>627</v>
@@ -8752,6 +8791,12 @@
       <c r="N25" t="s">
         <v>619</v>
       </c>
+      <c r="O25" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>620</v>
+      </c>
       <c r="Q25" t="s">
         <v>475</v>
       </c>
@@ -8759,13 +8804,13 @@
         <v>621</v>
       </c>
       <c r="V25">
-        <v>2300</v>
+        <v>15000</v>
       </c>
       <c r="W25">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X25">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="Y25">
         <v>0</v>
@@ -8777,10 +8822,10 @@
         <v>490</v>
       </c>
       <c r="AB25" s="3" t="s">
-        <v>528</v>
+        <v>479</v>
       </c>
       <c r="AC25" s="3" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="AE25" t="s">
         <v>492</v>
@@ -8796,6 +8841,9 @@
       </c>
       <c r="AM25" t="s">
         <v>483</v>
+      </c>
+      <c r="BG25" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="26" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -8806,16 +8854,16 @@
         <v>326</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D26">
-        <v>24424</v>
+        <v>24422</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I26" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="J26" t="s">
         <v>627</v>
@@ -8829,12 +8877,6 @@
       <c r="N26" t="s">
         <v>619</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="Q26" t="s">
         <v>475</v>
       </c>
@@ -8842,13 +8884,13 @@
         <v>621</v>
       </c>
       <c r="V26">
-        <v>3000</v>
+        <v>2300</v>
       </c>
       <c r="W26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X26">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Y26">
         <v>0</v>
@@ -8863,7 +8905,7 @@
         <v>528</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>622</v>
+        <v>636</v>
       </c>
       <c r="AE26" t="s">
         <v>492</v>
@@ -8879,9 +8921,6 @@
       </c>
       <c r="AM26" t="s">
         <v>483</v>
-      </c>
-      <c r="BG26" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="27" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -8892,13 +8931,13 @@
         <v>326</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D27">
-        <v>24426</v>
+        <v>24424</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="I27" t="s">
         <v>632</v>
@@ -8928,13 +8967,13 @@
         <v>621</v>
       </c>
       <c r="V27">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="W27">
         <v>5</v>
       </c>
       <c r="X27">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="Y27">
         <v>0</v>
@@ -8946,7 +8985,7 @@
         <v>490</v>
       </c>
       <c r="AB27" s="3" t="s">
-        <v>479</v>
+        <v>528</v>
       </c>
       <c r="AC27" s="3" t="s">
         <v>622</v>
@@ -8978,13 +9017,13 @@
         <v>326</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D28">
-        <v>24428</v>
+        <v>24426</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="I28" t="s">
         <v>632</v>
@@ -9014,13 +9053,13 @@
         <v>621</v>
       </c>
       <c r="V28">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="W28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="X28">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="Y28">
         <v>0</v>
@@ -9035,7 +9074,7 @@
         <v>479</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="AE28" t="s">
         <v>492</v>
@@ -9064,13 +9103,13 @@
         <v>326</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D29">
-        <v>24430</v>
+        <v>24428</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="I29" t="s">
         <v>632</v>
@@ -9100,13 +9139,13 @@
         <v>621</v>
       </c>
       <c r="V29">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="W29">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="X29">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="Y29">
         <v>0</v>
@@ -9118,10 +9157,10 @@
         <v>490</v>
       </c>
       <c r="AB29" s="3" t="s">
-        <v>528</v>
+        <v>479</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>622</v>
+        <v>636</v>
       </c>
       <c r="AE29" t="s">
         <v>492</v>
@@ -9150,16 +9189,16 @@
         <v>326</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D30">
-        <v>24432</v>
+        <v>24430</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="I30" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="J30" t="s">
         <v>627</v>
@@ -9173,6 +9212,12 @@
       <c r="N30" t="s">
         <v>619</v>
       </c>
+      <c r="O30" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>620</v>
+      </c>
       <c r="Q30" t="s">
         <v>475</v>
       </c>
@@ -9180,13 +9225,13 @@
         <v>621</v>
       </c>
       <c r="V30">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="W30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X30">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Y30">
         <v>0</v>
@@ -9217,6 +9262,9 @@
       </c>
       <c r="AM30" t="s">
         <v>483</v>
+      </c>
+      <c r="BG30" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="31" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -9227,16 +9275,16 @@
         <v>326</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D31">
-        <v>24434</v>
+        <v>24432</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="I31" t="s">
-        <v>632</v>
+        <v>647</v>
       </c>
       <c r="J31" t="s">
         <v>627</v>
@@ -9250,12 +9298,6 @@
       <c r="N31" t="s">
         <v>619</v>
       </c>
-      <c r="O31" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>620</v>
-      </c>
       <c r="Q31" t="s">
         <v>475</v>
       </c>
@@ -9263,13 +9305,13 @@
         <v>621</v>
       </c>
       <c r="V31">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="W31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y31">
         <v>0</v>
@@ -9300,9 +9342,6 @@
       </c>
       <c r="AM31" t="s">
         <v>483</v>
-      </c>
-      <c r="BG31" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="32" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -9313,16 +9352,16 @@
         <v>326</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D32">
-        <v>24436</v>
+        <v>24434</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="I32" t="s">
-        <v>652</v>
+        <v>632</v>
       </c>
       <c r="J32" t="s">
         <v>627</v>
@@ -9349,13 +9388,13 @@
         <v>621</v>
       </c>
       <c r="V32">
-        <v>6300</v>
+        <v>5000</v>
       </c>
       <c r="W32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X32">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="Y32">
         <v>0</v>
@@ -9370,7 +9409,7 @@
         <v>528</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="AE32" t="s">
         <v>492</v>
@@ -9388,7 +9427,7 @@
         <v>483</v>
       </c>
       <c r="BG32" t="s">
-        <v>139</v>
+        <v>623</v>
       </c>
     </row>
     <row r="33" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -9399,16 +9438,16 @@
         <v>326</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D33">
-        <v>24438</v>
+        <v>24436</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="I33" t="s">
-        <v>632</v>
+        <v>652</v>
       </c>
       <c r="J33" t="s">
         <v>627</v>
@@ -9435,13 +9474,13 @@
         <v>621</v>
       </c>
       <c r="V33">
-        <v>15000</v>
+        <v>6300</v>
       </c>
       <c r="W33">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="X33">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="Y33">
         <v>0</v>
@@ -9453,7 +9492,7 @@
         <v>490</v>
       </c>
       <c r="AB33" s="3" t="s">
-        <v>479</v>
+        <v>528</v>
       </c>
       <c r="AC33" s="3" t="s">
         <v>636</v>
@@ -9474,7 +9513,7 @@
         <v>483</v>
       </c>
       <c r="BG33" t="s">
-        <v>623</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:59" ht="365" x14ac:dyDescent="0.2">
@@ -9485,13 +9524,13 @@
         <v>326</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D34">
-        <v>24440</v>
+        <v>24438</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="I34" t="s">
         <v>632</v>
@@ -9521,13 +9560,13 @@
         <v>621</v>
       </c>
       <c r="V34">
-        <v>26000</v>
+        <v>15000</v>
       </c>
       <c r="W34">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="X34">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="Y34">
         <v>0</v>
@@ -9542,7 +9581,7 @@
         <v>479</v>
       </c>
       <c r="AC34" s="3" t="s">
-        <v>622</v>
+        <v>636</v>
       </c>
       <c r="AE34" t="s">
         <v>492</v>
@@ -9571,16 +9610,16 @@
         <v>326</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D35">
-        <v>24442</v>
+        <v>24440</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="I35" t="s">
-        <v>652</v>
+        <v>632</v>
       </c>
       <c r="J35" t="s">
         <v>627</v>
@@ -9607,13 +9646,13 @@
         <v>621</v>
       </c>
       <c r="V35">
-        <v>1000</v>
+        <v>26000</v>
       </c>
       <c r="W35">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="X35">
-        <v>150</v>
+        <v>2500</v>
       </c>
       <c r="Y35">
         <v>0</v>
@@ -9649,7 +9688,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="36" spans="1:59" ht="380" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:59" ht="365" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -9657,16 +9696,16 @@
         <v>326</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D36">
-        <v>24444</v>
+        <v>24442</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="I36" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="J36" t="s">
         <v>627</v>
@@ -9680,14 +9719,20 @@
       <c r="N36" t="s">
         <v>619</v>
       </c>
+      <c r="O36" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>620</v>
+      </c>
       <c r="Q36" t="s">
         <v>475</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>662</v>
+        <v>621</v>
       </c>
       <c r="V36">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="W36">
         <v>3</v>
@@ -9708,7 +9753,7 @@
         <v>479</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="AE36" t="s">
         <v>492</v>
@@ -9725,67 +9770,64 @@
       <c r="AM36" t="s">
         <v>483</v>
       </c>
+      <c r="BG36" t="s">
+        <v>623</v>
+      </c>
     </row>
-    <row r="37" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:59" ht="380" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D37">
-        <v>23746</v>
+        <v>24444</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="I37" t="s">
-        <v>665</v>
+        <v>661</v>
+      </c>
+      <c r="J37" t="s">
+        <v>627</v>
       </c>
       <c r="K37" t="s">
         <v>523</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="O37" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="P37" s="3" t="s">
-        <v>668</v>
+        <v>618</v>
+      </c>
+      <c r="N37" t="s">
+        <v>619</v>
       </c>
       <c r="Q37" t="s">
         <v>475</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="T37" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="U37" s="3" t="s">
-        <v>560</v>
+        <v>662</v>
       </c>
       <c r="V37">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="W37">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="X37">
-        <v>10000</v>
+        <v>150</v>
       </c>
       <c r="Y37">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Z37" t="s">
         <v>160</v>
       </c>
       <c r="AA37" t="s">
-        <v>670</v>
+        <v>490</v>
       </c>
       <c r="AB37" s="3" t="s">
         <v>479</v>
@@ -9797,7 +9839,7 @@
         <v>492</v>
       </c>
       <c r="AI37" t="s">
-        <v>535</v>
+        <v>481</v>
       </c>
       <c r="AJ37" t="s">
         <v>482</v>
@@ -9809,66 +9851,66 @@
         <v>483</v>
       </c>
     </row>
-    <row r="38" spans="1:59" ht="208" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="D38">
-        <v>24473</v>
+        <v>23746</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="I38" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="K38" t="s">
-        <v>606</v>
+        <v>523</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>577</v>
+        <v>666</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>595</v>
+        <v>668</v>
       </c>
       <c r="Q38" t="s">
-        <v>609</v>
+        <v>475</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>610</v>
+        <v>669</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="U38" s="3" t="s">
-        <v>527</v>
+        <v>560</v>
       </c>
       <c r="V38">
         <v>0</v>
       </c>
       <c r="W38">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="X38">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Y38">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="Z38" t="s">
         <v>160</v>
       </c>
       <c r="AA38" t="s">
-        <v>579</v>
+        <v>670</v>
       </c>
       <c r="AB38" s="3" t="s">
         <v>479</v>
@@ -9891,99 +9933,105 @@
       <c r="AM38" t="s">
         <v>483</v>
       </c>
-      <c r="BG38" t="s">
-        <v>139</v>
-      </c>
     </row>
-    <row r="39" spans="1:59" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:59" ht="208" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>102</v>
+        <v>671</v>
       </c>
       <c r="D39">
-        <v>24555</v>
+        <v>24473</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="I39" t="s">
+        <v>673</v>
+      </c>
+      <c r="K39" t="s">
+        <v>606</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>609</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>350</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>579</v>
+      </c>
+      <c r="AB39" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="AC39" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>492</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>535</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>482</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>483</v>
+      </c>
+      <c r="BG39" t="s">
+        <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:59" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>675</v>
+        <v>102</v>
       </c>
       <c r="D40">
-        <v>24871</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="I40" t="s">
-        <v>531</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>475</v>
-      </c>
-      <c r="S40" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="T40" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="U40" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>0</v>
-      </c>
-      <c r="X40">
-        <v>0</v>
-      </c>
-      <c r="Y40">
-        <v>0</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>482</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>490</v>
-      </c>
-      <c r="AB40" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="AC40" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="AE40" t="s">
-        <v>492</v>
-      </c>
-      <c r="AI40" t="s">
-        <v>481</v>
-      </c>
-      <c r="AJ40" t="s">
-        <v>482</v>
-      </c>
-      <c r="AK40" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>483</v>
+        <v>24555</v>
       </c>
     </row>
     <row r="41" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
@@ -9994,25 +10042,19 @@
         <v>360</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D41">
-        <v>24873</v>
+        <v>24871</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="I41" t="s">
         <v>531</v>
       </c>
-      <c r="K41" t="s">
-        <v>138</v>
-      </c>
-      <c r="L41" t="s">
-        <v>680</v>
-      </c>
       <c r="M41" s="3" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="O41" s="3" t="s">
         <v>517</v>
@@ -10051,7 +10093,7 @@
         <v>528</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>512</v>
+        <v>636</v>
       </c>
       <c r="AE41" t="s">
         <v>492</v>
@@ -10077,13 +10119,13 @@
         <v>360</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="D42">
-        <v>24875</v>
+        <v>24873</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="I42" t="s">
         <v>531</v>
@@ -10092,10 +10134,10 @@
         <v>138</v>
       </c>
       <c r="L42" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="O42" s="3" t="s">
         <v>517</v>
@@ -10134,7 +10176,7 @@
         <v>528</v>
       </c>
       <c r="AC42" s="3" t="s">
-        <v>636</v>
+        <v>512</v>
       </c>
       <c r="AE42" t="s">
         <v>492</v>
@@ -10160,25 +10202,25 @@
         <v>360</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="D43">
-        <v>24877</v>
+        <v>24875</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="I43" t="s">
-        <v>688</v>
+        <v>531</v>
       </c>
       <c r="K43" t="s">
         <v>138</v>
       </c>
       <c r="L43" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="O43" s="3" t="s">
         <v>517</v>
@@ -10220,7 +10262,7 @@
         <v>636</v>
       </c>
       <c r="AE43" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="AI43" t="s">
         <v>481</v>
@@ -10240,31 +10282,31 @@
         <v>83</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D44">
-        <v>24507</v>
+        <v>24877</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="I44" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="K44" t="s">
-        <v>523</v>
+        <v>138</v>
+      </c>
+      <c r="L44" t="s">
+        <v>689</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>690</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>694</v>
+        <v>517</v>
       </c>
       <c r="Q44" t="s">
         <v>475</v>
@@ -10276,22 +10318,22 @@
         <v>502</v>
       </c>
       <c r="U44" s="3" t="s">
-        <v>527</v>
+        <v>478</v>
       </c>
       <c r="V44">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="W44">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="X44">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="Y44">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="Z44" t="s">
-        <v>160</v>
+        <v>482</v>
       </c>
       <c r="AA44" t="s">
         <v>490</v>
@@ -10300,10 +10342,10 @@
         <v>528</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>695</v>
+        <v>636</v>
       </c>
       <c r="AE44" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="AI44" t="s">
         <v>481</v>
@@ -10316,9 +10358,6 @@
       </c>
       <c r="AM44" t="s">
         <v>483</v>
-      </c>
-      <c r="BG44" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="45" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
@@ -10326,67 +10365,70 @@
         <v>83</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="D45">
-        <v>24558</v>
+        <v>24507</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="I45" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="K45" t="s">
-        <v>700</v>
+        <v>523</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>517</v>
+        <v>543</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>694</v>
       </c>
       <c r="Q45" t="s">
         <v>475</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>702</v>
+        <v>476</v>
       </c>
       <c r="T45" s="3" t="s">
         <v>502</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>478</v>
+        <v>527</v>
       </c>
       <c r="V45">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="W45">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X45">
-        <v>700</v>
+        <v>6000</v>
       </c>
       <c r="Y45">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="Z45" t="s">
         <v>160</v>
       </c>
       <c r="AA45" t="s">
-        <v>561</v>
+        <v>490</v>
       </c>
       <c r="AB45" s="3" t="s">
         <v>528</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>480</v>
+        <v>695</v>
       </c>
       <c r="AE45" t="s">
-        <v>492</v>
+        <v>534</v>
       </c>
       <c r="AI45" t="s">
         <v>481</v>
@@ -10399,6 +10441,9 @@
       </c>
       <c r="AM45" t="s">
         <v>483</v>
+      </c>
+      <c r="BG45" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="46" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
@@ -10409,22 +10454,22 @@
         <v>365</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="D46">
-        <v>24560</v>
+        <v>24558</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="I46" t="s">
         <v>699</v>
       </c>
       <c r="K46" t="s">
-        <v>523</v>
+        <v>700</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="O46" s="3" t="s">
         <v>517</v>
@@ -10448,10 +10493,10 @@
         <v>0</v>
       </c>
       <c r="X46">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="Y46">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Z46" t="s">
         <v>160</v>
@@ -10459,8 +10504,11 @@
       <c r="AA46" t="s">
         <v>561</v>
       </c>
+      <c r="AB46" s="3" t="s">
+        <v>528</v>
+      </c>
       <c r="AC46" s="3" t="s">
-        <v>706</v>
+        <v>480</v>
       </c>
       <c r="AE46" t="s">
         <v>492</v>
@@ -10478,7 +10526,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="47" spans="1:59" ht="350" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -10486,13 +10534,13 @@
         <v>365</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D47">
-        <v>24562</v>
+        <v>24560</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="I47" t="s">
         <v>699</v>
@@ -10501,7 +10549,7 @@
         <v>523</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="O47" s="3" t="s">
         <v>517</v>
@@ -10510,7 +10558,7 @@
         <v>475</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>596</v>
+        <v>702</v>
       </c>
       <c r="T47" s="3" t="s">
         <v>502</v>
@@ -10519,7 +10567,7 @@
         <v>478</v>
       </c>
       <c r="V47">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="W47">
         <v>0</v>
@@ -10528,7 +10576,7 @@
         <v>100</v>
       </c>
       <c r="Y47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Z47" t="s">
         <v>160</v>
@@ -10536,11 +10584,8 @@
       <c r="AA47" t="s">
         <v>561</v>
       </c>
-      <c r="AB47" s="3" t="s">
-        <v>528</v>
-      </c>
       <c r="AC47" s="3" t="s">
-        <v>480</v>
+        <v>706</v>
       </c>
       <c r="AE47" t="s">
         <v>492</v>
@@ -10558,27 +10603,30 @@
         <v>483</v>
       </c>
     </row>
-    <row r="48" spans="1:59" ht="160" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:59" ht="350" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D48">
-        <v>24833</v>
+        <v>24562</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="I48" t="s">
-        <v>712</v>
+        <v>699</v>
+      </c>
+      <c r="K48" t="s">
+        <v>523</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="O48" s="3" t="s">
         <v>517</v>
@@ -10587,40 +10635,43 @@
         <v>475</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>714</v>
+        <v>596</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>478</v>
       </c>
       <c r="V48">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="W48">
         <v>0</v>
       </c>
       <c r="X48">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z48" t="s">
         <v>160</v>
       </c>
       <c r="AA48" t="s">
-        <v>579</v>
+        <v>561</v>
       </c>
       <c r="AB48" s="3" t="s">
-        <v>568</v>
+        <v>528</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>715</v>
+        <v>480</v>
       </c>
       <c r="AE48" t="s">
         <v>492</v>
       </c>
       <c r="AI48" t="s">
-        <v>716</v>
+        <v>481</v>
       </c>
       <c r="AJ48" t="s">
         <v>482</v>
@@ -10632,30 +10683,27 @@
         <v>483</v>
       </c>
     </row>
-    <row r="49" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:59" ht="160" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>83</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="D49">
-        <v>24480</v>
+        <v>24833</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="I49" t="s">
-        <v>719</v>
-      </c>
-      <c r="K49" t="s">
-        <v>606</v>
+        <v>712</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="O49" s="3" t="s">
         <v>517</v>
@@ -10664,19 +10712,19 @@
         <v>475</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>476</v>
+        <v>714</v>
       </c>
       <c r="V49">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="W49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X49">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="Y49">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Z49" t="s">
         <v>160</v>
@@ -10685,16 +10733,19 @@
         <v>579</v>
       </c>
       <c r="AB49" s="3" t="s">
-        <v>721</v>
+        <v>568</v>
       </c>
       <c r="AC49" s="3" t="s">
-        <v>636</v>
+        <v>138</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>715</v>
       </c>
       <c r="AE49" t="s">
         <v>492</v>
       </c>
       <c r="AI49" t="s">
-        <v>481</v>
+        <v>716</v>
       </c>
       <c r="AJ49" t="s">
         <v>482</v>
@@ -10704,9 +10755,6 @@
       </c>
       <c r="AM49" t="s">
         <v>483</v>
-      </c>
-      <c r="BG49" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="50" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
@@ -10714,64 +10762,58 @@
         <v>83</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="D50">
-        <v>23754</v>
+        <v>24480</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="I50" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="K50" t="s">
-        <v>523</v>
+        <v>606</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>727</v>
+        <v>517</v>
       </c>
       <c r="Q50" t="s">
         <v>475</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="T50" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="U50" s="3" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="V50">
-        <v>75</v>
+        <v>1000</v>
       </c>
       <c r="W50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X50">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="Y50">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="Z50" t="s">
         <v>160</v>
       </c>
       <c r="AA50" t="s">
-        <v>728</v>
+        <v>579</v>
       </c>
       <c r="AB50" s="3" t="s">
-        <v>528</v>
+        <v>721</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>695</v>
+        <v>636</v>
       </c>
       <c r="AE50" t="s">
         <v>492</v>
@@ -10789,57 +10831,66 @@
         <v>483</v>
       </c>
       <c r="BG50" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
     </row>
-    <row r="51" spans="1:59" ht="380" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:59" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="D51">
-        <v>23774</v>
+        <v>23754</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="I51" t="s">
-        <v>732</v>
+        <v>725</v>
+      </c>
+      <c r="K51" t="s">
+        <v>523</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>516</v>
+        <v>726</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>517</v>
+        <v>727</v>
       </c>
       <c r="Q51" t="s">
         <v>475</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>733</v>
+        <v>545</v>
+      </c>
+      <c r="T51" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>478</v>
       </c>
       <c r="V51">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="W51">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="X51">
-        <v>450</v>
+        <v>80</v>
       </c>
       <c r="Y51">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="Z51" t="s">
         <v>160</v>
       </c>
       <c r="AA51" t="s">
-        <v>490</v>
+        <v>728</v>
       </c>
       <c r="AB51" s="3" t="s">
         <v>528</v>
@@ -10860,6 +10911,80 @@
         <v>126</v>
       </c>
       <c r="AM51" t="s">
+        <v>483</v>
+      </c>
+      <c r="BG51" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="52" spans="1:59" ht="380" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="D52">
+        <v>23774</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="I52" t="s">
+        <v>732</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>475</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="V52">
+        <v>100</v>
+      </c>
+      <c r="W52">
+        <v>25</v>
+      </c>
+      <c r="X52">
+        <v>450</v>
+      </c>
+      <c r="Y52">
+        <v>65</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>490</v>
+      </c>
+      <c r="AB52" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="AC52" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>492</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>481</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>482</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM52" t="s">
         <v>483</v>
       </c>
     </row>

</xml_diff>